<commit_message>
working model for all tiers
</commit_message>
<xml_diff>
--- a/Data_inputs/PSERS_PlanInfo_AV2015.xlsx
+++ b/Data_inputs/PSERS_PlanInfo_AV2015.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="853" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="853" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="31" r:id="rId1"/>
@@ -2759,15 +2759,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>570843</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>361293</xdr:colOff>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>112702</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2791,7 +2791,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5676900" y="857250"/>
+          <a:off x="590550" y="666750"/>
           <a:ext cx="5257143" cy="12780952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8113,8 +8113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10254,8 +10254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="S72" sqref="S72"/>
+    <sheetView tabSelected="1" topLeftCell="N2" workbookViewId="0">
+      <selection activeCell="AC4" sqref="AC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10370,7 +10370,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>